<commit_message>
program ZTH Andrei Marica
</commit_message>
<xml_diff>
--- a/Program+Traineri_Z2H_2017.xlsx
+++ b/Program+Traineri_Z2H_2017.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Know your language - OOP</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Asistenti</t>
+  </si>
+  <si>
+    <t>AndreiMarica(?)</t>
+  </si>
+  <si>
+    <t>AndreiMarica</t>
   </si>
 </sst>
 </file>
@@ -498,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -593,7 +599,9 @@
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
     </row>
@@ -605,7 +613,9 @@
         <v>2</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -616,7 +626,9 @@
         <v>3</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -693,7 +705,9 @@
         <v>8</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -704,7 +718,9 @@
         <v>9</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -715,7 +731,9 @@
         <v>10</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -726,7 +744,9 @@
         <v>11</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>